<commit_message>
updated scripts and some dfs
</commit_message>
<xml_diff>
--- a/data/raw_data/Midstory Removal/Plot Info.xlsx
+++ b/data/raw_data/Midstory Removal/Plot Info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/smc0124_auburn_edu/Documents/Desktop/Auburn/FireMS/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tigermailauburn-my.sharepoint.com/personal/smc0124_auburn_edu/Documents/Desktop/AuburnMS/data/raw_data/Midstory Removal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{62E8CCB8-2239-4CBD-9D39-903FDEDAD310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C76853B-96A8-4997-AACB-76607CF46DF4}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{62E8CCB8-2239-4CBD-9D39-903FDEDAD310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F37A629-9557-41FF-95C8-63640E783661}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A12F37A-F2A8-4CC7-95F1-82C3664AAEB7}"/>
   </bookViews>
@@ -34,16 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
-  <si>
-    <t>plot</t>
-  </si>
-  <si>
-    <t>meso_os</t>
-  </si>
-  <si>
-    <t>canopy_try</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t>high</t>
   </si>
@@ -54,7 +45,13 @@
     <t>low</t>
   </si>
   <si>
-    <t xml:space="preserve">RAIN LOGGER </t>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Meso_OS_BAsqft</t>
   </si>
 </sst>
 </file>
@@ -406,26 +403,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3D5C56-A9F2-421A-A270-97C4BD44CBEE}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -433,115 +433,109 @@
         <v>87</v>
       </c>
       <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>84.3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B4">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>52.2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>47.9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>41.1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>61</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B4">
+      <c r="B10">
         <v>83.6</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>66.400000000000006</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="B11">
         <v>64.900000000000006</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>64.400000000000006</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10">
-        <v>52.2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>47.9</v>
-      </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -549,26 +543,23 @@
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>41.1</v>
+        <v>84.3</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C13">
-    <sortCondition descending="1" ref="B1:B13"/>
+    <sortCondition ref="A1:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>